<commit_message>
complete date and commitee
</commit_message>
<xml_diff>
--- a/tools/commiteeMembers.xlsx
+++ b/tools/commiteeMembers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leyau\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DD0FF5-68D0-41E9-97D9-E717982066D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2A4135-1787-45F4-A9D0-B916073432D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="953">
   <si>
     <t>#</t>
   </si>
@@ -2700,6 +2700,196 @@
   </si>
   <si>
     <t>https://scholar.googleusercontent.com/citations?view_op=view_photo&amp;user=Wuq5F8MAAAAJ&amp;citpid=2</t>
+  </si>
+  <si>
+    <t>https://scholar.google.it/citations?user=8Z20aIMAAAAJ&amp;hl=it</t>
+  </si>
+  <si>
+    <t>https://apps.ualberta.ca/directory/person/bezemer</t>
+  </si>
+  <si>
+    <t>https://www.monash.edu/it/humanise-lab/about-us/our-students/current-monash-students/tingtin-bi</t>
+  </si>
+  <si>
+    <t>https://research.jetbrains.org/researchers/timofey.bryksin/</t>
+  </si>
+  <si>
+    <t>https://jinfuchen.github.io/jinfu/</t>
+  </si>
+  <si>
+    <t>https://cs.nju.edu.cn/chenlin/index.htm</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/site/ejchoi710/</t>
+  </si>
+  <si>
+    <t>https://informatics.tuwien.ac.at/people/juergen-cito</t>
+  </si>
+  <si>
+    <t>https://www.cs.usask.ca/faculty/zadiacodabux/</t>
+  </si>
+  <si>
+    <t>https://wwwfr.uni.lu/layout/set/print/snt/people/maxime_cordy</t>
+  </si>
+  <si>
+    <t>https://www.brunel.ac.uk/people/steve-counsell</t>
+  </si>
+  <si>
+    <t>https://diegoeliascosta.github.io/</t>
+  </si>
+  <si>
+    <t>https://www.uni-trier.de/index.php?id=3569</t>
+  </si>
+  <si>
+    <t>https://xiaoningdu.github.io/</t>
+  </si>
+  <si>
+    <t>https://www.cristal.univ-lille.fr/~etien/</t>
+  </si>
+  <si>
+    <t>https://cse.umn.edu/cs/mattia-fazzini</t>
+  </si>
+  <si>
+    <t>https://fengyang-nju.github.io/</t>
+  </si>
+  <si>
+    <t>https://dfucci.github.io/</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/view/sanondagupta147/sanonda-datta-gupta</t>
+  </si>
+  <si>
+    <t>https://gyimothy.sed.hu/</t>
+  </si>
+  <si>
+    <t>https://habchisarra.github.io/</t>
+  </si>
+  <si>
+    <t>https://pinjiahe.github.io/</t>
+  </si>
+  <si>
+    <t>http://hematimoghadam.faculty.vru.ac.ir/?part=menu&amp;inc=menu&amp;id=118</t>
+  </si>
+  <si>
+    <t>https://cmps.ok.ubc.ca/about/contact/fatemeh-hendijani-fard/</t>
+  </si>
+  <si>
+    <t>https://xing-hu.github.io/</t>
+  </si>
+  <si>
+    <t>http://sei.buaa.edu.cn/info/1082/1121.htm</t>
+  </si>
+  <si>
+    <t>https://kanghj.github.io/</t>
+  </si>
+  <si>
+    <t>NULL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://mkechagia.github.io/</t>
+  </si>
+  <si>
+    <t>https://researchers.uq.edu.au/researcher/30167</t>
+  </si>
+  <si>
+    <t>https://vovak.me/</t>
+  </si>
+  <si>
+    <t>https://raux.github.io/</t>
+  </si>
+  <si>
+    <t>https://lamothemax.github.io/</t>
+  </si>
+  <si>
+    <t>http://www.cse.cqu.edu.cn/info/2096/4505.htm</t>
+  </si>
+  <si>
+    <t>http://sei.pku.edu.cn/~lige/</t>
+  </si>
+  <si>
+    <t>https://lilicoding.github.io/</t>
+  </si>
+  <si>
+    <t>https://lx0704.github.io/</t>
+  </si>
+  <si>
+    <t>https://binlin.info/</t>
+  </si>
+  <si>
+    <t>https://liuhuigmail.github.io/</t>
+  </si>
+  <si>
+    <t>https://person.zju.edu.cn/en/liuzhongxin</t>
+  </si>
+  <si>
+    <t>https://yilinglou.github.io/</t>
+  </si>
+  <si>
+    <t>https://www4.comp.polyu.edu.hk/~csxluo/</t>
+  </si>
+  <si>
+    <t>https://mkaouer.net/author/mohamed-wiem-mkaouer/</t>
+  </si>
+  <si>
+    <t>http://www.ranmo.site/</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/site/ouniaali/home</t>
+  </si>
+  <si>
+    <t>https://lucapascarella.com/</t>
+  </si>
+  <si>
+    <t>https://collab.di.uniba.it/luigi-quaranta/</t>
+  </si>
+  <si>
+    <t>https://www.fujitsu.com/us/about/businesspolicy/tech/rd/research-staff/ripon.html</t>
+  </si>
+  <si>
+    <t>https://msayagh.github.io/</t>
+  </si>
+  <si>
+    <t>https://allisonius.github.io/</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=PIBtljkAAAAJ&amp;hl=zh-CN</t>
+  </si>
+  <si>
+    <t>https://home.cse.ust.hk/~shuaiw/</t>
+  </si>
+  <si>
+    <t>https://wangying-neu.github.io/</t>
+  </si>
+  <si>
+    <t>https://people.ucas.ac.cn/~weijun</t>
+  </si>
+  <si>
+    <t>https://faculty.stevens.edu/lxiao6</t>
+  </si>
+  <si>
+    <t>https://xiaoyuanxie.github.io/</t>
+  </si>
+  <si>
+    <t>http://www.cse.cqu.edu.cn/info/2095/5040.htm</t>
+  </si>
+  <si>
+    <t>https://jinqiuyang.github.io/</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=-qRba7AAAAAJ&amp;hl=it</t>
+  </si>
+  <si>
+    <t>https://www.cs.sjtu.edu.cn/~zhonghao/</t>
+  </si>
+  <si>
+    <t>http://yiikou.com/jiayuan/about/</t>
+  </si>
+  <si>
+    <t>https://www.eecg.utoronto.ca/~shuruiz/</t>
+  </si>
+  <si>
+    <t>http://faculty.nuaa.edu.cn/zhouyu/en/index.htm</t>
   </si>
 </sst>
 </file>
@@ -3249,8 +3439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I169" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="L177" sqref="L177"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H181" sqref="H181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3261,11 +3451,11 @@
     <col min="5" max="5" width="32.42578125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="60" customWidth="1"/>
-    <col min="8" max="8" width="52.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="2" customWidth="1"/>
+    <col min="8" max="8" width="134.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="96.85546875" customWidth="1"/>
+    <col min="12" max="12" width="98.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="44.25" x14ac:dyDescent="0.2">
@@ -3404,7 +3594,9 @@
       <c r="G4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>890</v>
+      </c>
       <c r="I4" s="5" t="s">
         <v>16</v>
       </c>
@@ -3554,7 +3746,9 @@
       <c r="G8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>891</v>
+      </c>
       <c r="I8" s="5" t="s">
         <v>16</v>
       </c>
@@ -3590,7 +3784,9 @@
       <c r="G9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>892</v>
+      </c>
       <c r="I9" s="6" t="s">
         <v>16</v>
       </c>
@@ -3664,7 +3860,9 @@
       <c r="G11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>893</v>
+      </c>
       <c r="I11" s="6" t="s">
         <v>16</v>
       </c>
@@ -4004,7 +4202,9 @@
       <c r="G20" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H20" s="4"/>
+      <c r="H20" s="4" t="s">
+        <v>894</v>
+      </c>
       <c r="I20" s="5" t="s">
         <v>16</v>
       </c>
@@ -4078,7 +4278,9 @@
       <c r="G22" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>895</v>
+      </c>
       <c r="I22" s="5" t="s">
         <v>16</v>
       </c>
@@ -4152,7 +4354,9 @@
       <c r="G24" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="4" t="s">
+        <v>896</v>
+      </c>
       <c r="I24" s="5" t="s">
         <v>16</v>
       </c>
@@ -4188,7 +4392,9 @@
       <c r="G25" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="H25" s="3"/>
+      <c r="H25" s="3" t="s">
+        <v>897</v>
+      </c>
       <c r="I25" s="6" t="s">
         <v>16</v>
       </c>
@@ -4262,7 +4468,9 @@
       <c r="G27" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="H27" s="3"/>
+      <c r="H27" s="3" t="s">
+        <v>898</v>
+      </c>
       <c r="I27" s="6" t="s">
         <v>16</v>
       </c>
@@ -4298,7 +4506,9 @@
       <c r="G28" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>899</v>
+      </c>
       <c r="I28" s="5" t="s">
         <v>16</v>
       </c>
@@ -4372,7 +4582,9 @@
       <c r="G30" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H30" s="4"/>
+      <c r="H30" s="4" t="s">
+        <v>900</v>
+      </c>
       <c r="I30" s="5" t="s">
         <v>16</v>
       </c>
@@ -4408,7 +4620,9 @@
       <c r="G31" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H31" s="3"/>
+      <c r="H31" s="3" t="s">
+        <v>901</v>
+      </c>
       <c r="I31" s="6" t="s">
         <v>16</v>
       </c>
@@ -4444,7 +4658,9 @@
       <c r="G32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="4"/>
+      <c r="H32" s="4" t="s">
+        <v>901</v>
+      </c>
       <c r="I32" s="5" t="s">
         <v>16</v>
       </c>
@@ -4708,7 +4924,9 @@
       <c r="G39" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="H39" s="3"/>
+      <c r="H39" s="3" t="s">
+        <v>902</v>
+      </c>
       <c r="I39" s="6" t="s">
         <v>16</v>
       </c>
@@ -4782,7 +5000,9 @@
       <c r="G41" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H41" s="3"/>
+      <c r="H41" s="3" t="s">
+        <v>903</v>
+      </c>
       <c r="I41" s="6" t="s">
         <v>16</v>
       </c>
@@ -4894,7 +5114,9 @@
       <c r="G44" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="H44" s="4"/>
+      <c r="H44" s="4" t="s">
+        <v>904</v>
+      </c>
       <c r="I44" s="5" t="s">
         <v>16</v>
       </c>
@@ -4930,7 +5152,9 @@
       <c r="G45" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H45" s="3"/>
+      <c r="H45" s="3" t="s">
+        <v>905</v>
+      </c>
       <c r="I45" s="6" t="s">
         <v>16</v>
       </c>
@@ -4966,7 +5190,9 @@
       <c r="G46" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="H46" s="4"/>
+      <c r="H46" s="4" t="s">
+        <v>906</v>
+      </c>
       <c r="I46" s="5" t="s">
         <v>16</v>
       </c>
@@ -5040,7 +5266,9 @@
       <c r="G48" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="H48" s="4"/>
+      <c r="H48" s="4" t="s">
+        <v>907</v>
+      </c>
       <c r="I48" s="5" t="s">
         <v>16</v>
       </c>
@@ -5304,7 +5532,9 @@
       <c r="G55" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="H55" s="3"/>
+      <c r="H55" s="3" t="s">
+        <v>908</v>
+      </c>
       <c r="I55" s="6" t="s">
         <v>16</v>
       </c>
@@ -5340,7 +5570,9 @@
       <c r="G56" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="H56" s="4"/>
+      <c r="H56" s="4" t="s">
+        <v>909</v>
+      </c>
       <c r="I56" s="5" t="s">
         <v>16</v>
       </c>
@@ -5376,7 +5608,9 @@
       <c r="G57" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="H57" s="3"/>
+      <c r="H57" s="3" t="s">
+        <v>910</v>
+      </c>
       <c r="I57" s="6" t="s">
         <v>16</v>
       </c>
@@ -5488,7 +5722,9 @@
       <c r="G60" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="H60" s="4"/>
+      <c r="H60" s="4" t="s">
+        <v>911</v>
+      </c>
       <c r="I60" s="5" t="s">
         <v>16</v>
       </c>
@@ -5524,7 +5760,9 @@
       <c r="G61" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="H61" s="3"/>
+      <c r="H61" s="3" t="s">
+        <v>911</v>
+      </c>
       <c r="I61" s="6" t="s">
         <v>16</v>
       </c>
@@ -5560,7 +5798,9 @@
       <c r="G62" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="H62" s="4"/>
+      <c r="H62" s="4" t="s">
+        <v>912</v>
+      </c>
       <c r="I62" s="5" t="s">
         <v>16</v>
       </c>
@@ -5596,7 +5836,9 @@
       <c r="G63" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="H63" s="3"/>
+      <c r="H63" s="3" t="s">
+        <v>913</v>
+      </c>
       <c r="I63" s="6" t="s">
         <v>16</v>
       </c>
@@ -5784,7 +6026,9 @@
       <c r="G68" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H68" s="4"/>
+      <c r="H68" s="4" t="s">
+        <v>914</v>
+      </c>
       <c r="I68" s="5" t="s">
         <v>16</v>
       </c>
@@ -5932,7 +6176,9 @@
       <c r="G72" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="H72" s="4"/>
+      <c r="H72" s="4" t="s">
+        <v>915</v>
+      </c>
       <c r="I72" s="5" t="s">
         <v>16</v>
       </c>
@@ -6006,7 +6252,9 @@
       <c r="G74" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="H74" s="14"/>
+      <c r="H74" s="14" t="s">
+        <v>917</v>
+      </c>
       <c r="I74" s="15" t="s">
         <v>16</v>
       </c>
@@ -6118,7 +6366,9 @@
       <c r="G77" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="H77" s="3"/>
+      <c r="H77" s="3" t="s">
+        <v>916</v>
+      </c>
       <c r="I77" s="6" t="s">
         <v>16</v>
       </c>
@@ -6230,7 +6480,9 @@
       <c r="G80" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="H80" s="4"/>
+      <c r="H80" s="4" t="s">
+        <v>918</v>
+      </c>
       <c r="I80" s="5" t="s">
         <v>16</v>
       </c>
@@ -6342,7 +6594,9 @@
       <c r="G83" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="H83" s="3"/>
+      <c r="H83" s="3" t="s">
+        <v>919</v>
+      </c>
       <c r="I83" s="6" t="s">
         <v>16</v>
       </c>
@@ -6378,7 +6632,9 @@
       <c r="G84" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H84" s="4"/>
+      <c r="H84" s="4" t="s">
+        <v>920</v>
+      </c>
       <c r="I84" s="5" t="s">
         <v>16</v>
       </c>
@@ -6414,7 +6670,9 @@
       <c r="G85" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H85" s="3"/>
+      <c r="H85" s="3" t="s">
+        <v>920</v>
+      </c>
       <c r="I85" s="6" t="s">
         <v>16</v>
       </c>
@@ -6488,7 +6746,9 @@
       <c r="G87" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="H87" s="3"/>
+      <c r="H87" s="3" t="s">
+        <v>921</v>
+      </c>
       <c r="I87" s="6" t="s">
         <v>16</v>
       </c>
@@ -6524,7 +6784,9 @@
       <c r="G88" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="H88" s="4"/>
+      <c r="H88" s="4" t="s">
+        <v>922</v>
+      </c>
       <c r="I88" s="5" t="s">
         <v>16</v>
       </c>
@@ -6560,7 +6822,9 @@
       <c r="G89" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="H89" s="3"/>
+      <c r="H89" s="3" t="s">
+        <v>922</v>
+      </c>
       <c r="I89" s="6" t="s">
         <v>16</v>
       </c>
@@ -6634,7 +6898,9 @@
       <c r="G91" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="H91" s="3"/>
+      <c r="H91" s="3" t="s">
+        <v>923</v>
+      </c>
       <c r="I91" s="6" t="s">
         <v>16</v>
       </c>
@@ -6708,7 +6974,9 @@
       <c r="G93" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="H93" s="3"/>
+      <c r="H93" s="3" t="s">
+        <v>924</v>
+      </c>
       <c r="I93" s="6" t="s">
         <v>16</v>
       </c>
@@ -6744,7 +7012,9 @@
       <c r="G94" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H94" s="4"/>
+      <c r="H94" s="4" t="s">
+        <v>925</v>
+      </c>
       <c r="I94" s="5" t="s">
         <v>16</v>
       </c>
@@ -6780,7 +7050,9 @@
       <c r="G95" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H95" s="3"/>
+      <c r="H95" s="3" t="s">
+        <v>925</v>
+      </c>
       <c r="I95" s="6" t="s">
         <v>398</v>
       </c>
@@ -6816,7 +7088,9 @@
       <c r="G96" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="H96" s="4"/>
+      <c r="H96" s="4" t="s">
+        <v>926</v>
+      </c>
       <c r="I96" s="5" t="s">
         <v>16</v>
       </c>
@@ -6852,7 +7126,9 @@
       <c r="G97" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="H97" s="3"/>
+      <c r="H97" s="3" t="s">
+        <v>927</v>
+      </c>
       <c r="I97" s="6" t="s">
         <v>16</v>
       </c>
@@ -6926,7 +7202,9 @@
       <c r="G99" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="H99" s="3"/>
+      <c r="H99" s="3" t="s">
+        <v>928</v>
+      </c>
       <c r="I99" s="6" t="s">
         <v>16</v>
       </c>
@@ -6962,7 +7240,9 @@
       <c r="G100" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H100" s="4"/>
+      <c r="H100" s="4" t="s">
+        <v>929</v>
+      </c>
       <c r="I100" s="5" t="s">
         <v>16</v>
       </c>
@@ -6998,7 +7278,9 @@
       <c r="G101" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H101" s="3"/>
+      <c r="H101" s="3" t="s">
+        <v>929</v>
+      </c>
       <c r="I101" s="6" t="s">
         <v>16</v>
       </c>
@@ -7110,7 +7392,9 @@
       <c r="G104" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="H104" s="4"/>
+      <c r="H104" s="4" t="s">
+        <v>930</v>
+      </c>
       <c r="I104" s="5" t="s">
         <v>16</v>
       </c>
@@ -7146,7 +7430,9 @@
       <c r="G105" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="H105" s="3"/>
+      <c r="H105" s="3" t="s">
+        <v>931</v>
+      </c>
       <c r="I105" s="6" t="s">
         <v>398</v>
       </c>
@@ -7372,7 +7658,9 @@
       <c r="G111" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="H111" s="3"/>
+      <c r="H111" s="3" t="s">
+        <v>932</v>
+      </c>
       <c r="I111" s="6" t="s">
         <v>16</v>
       </c>
@@ -7408,7 +7696,9 @@
       <c r="G112" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="H112" s="4"/>
+      <c r="H112" s="4" t="s">
+        <v>933</v>
+      </c>
       <c r="I112" s="5" t="s">
         <v>16</v>
       </c>
@@ -7748,7 +8038,9 @@
       <c r="G121" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="H121" s="3"/>
+      <c r="H121" s="3" t="s">
+        <v>934</v>
+      </c>
       <c r="I121" s="6" t="s">
         <v>16</v>
       </c>
@@ -7860,7 +8152,9 @@
       <c r="G124" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="H124" s="4"/>
+      <c r="H124" s="4" t="s">
+        <v>935</v>
+      </c>
       <c r="I124" s="5" t="s">
         <v>16</v>
       </c>
@@ -8010,7 +8304,9 @@
       <c r="G128" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="H128" s="4"/>
+      <c r="H128" s="4" t="s">
+        <v>936</v>
+      </c>
       <c r="I128" s="5" t="s">
         <v>16</v>
       </c>
@@ -8312,7 +8608,9 @@
       <c r="G136" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="H136" s="4"/>
+      <c r="H136" s="4" t="s">
+        <v>937</v>
+      </c>
       <c r="I136" s="5" t="s">
         <v>16</v>
       </c>
@@ -8348,7 +8646,9 @@
       <c r="G137" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="H137" s="3"/>
+      <c r="H137" s="3" t="s">
+        <v>938</v>
+      </c>
       <c r="I137" s="6" t="s">
         <v>16</v>
       </c>
@@ -8574,7 +8874,9 @@
       <c r="G143" s="3" t="s">
         <v>607</v>
       </c>
-      <c r="H143" s="3"/>
+      <c r="H143" s="3" t="s">
+        <v>939</v>
+      </c>
       <c r="I143" s="6" t="s">
         <v>16</v>
       </c>
@@ -8800,7 +9102,9 @@
       <c r="G149" s="3" t="s">
         <v>636</v>
       </c>
-      <c r="H149" s="3"/>
+      <c r="H149" s="3" t="s">
+        <v>940</v>
+      </c>
       <c r="I149" s="6" t="s">
         <v>16</v>
       </c>
@@ -8836,7 +9140,9 @@
       <c r="G150" s="4" t="s">
         <v>639</v>
       </c>
-      <c r="H150" s="4"/>
+      <c r="H150" s="4" t="s">
+        <v>941</v>
+      </c>
       <c r="I150" s="5" t="s">
         <v>16</v>
       </c>
@@ -8910,7 +9216,9 @@
       <c r="G152" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="H152" s="4"/>
+      <c r="H152" s="4" t="s">
+        <v>942</v>
+      </c>
       <c r="I152" s="5" t="s">
         <v>398</v>
       </c>
@@ -8946,7 +9254,9 @@
       <c r="G153" s="3" t="s">
         <v>650</v>
       </c>
-      <c r="H153" s="3"/>
+      <c r="H153" s="3" t="s">
+        <v>943</v>
+      </c>
       <c r="I153" s="6" t="s">
         <v>16</v>
       </c>
@@ -9058,7 +9368,9 @@
       <c r="G156" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="H156" s="4"/>
+      <c r="H156" s="4" t="s">
+        <v>944</v>
+      </c>
       <c r="I156" s="5" t="s">
         <v>16</v>
       </c>
@@ -9132,7 +9444,9 @@
       <c r="G158" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="H158" s="4"/>
+      <c r="H158" s="4" t="s">
+        <v>945</v>
+      </c>
       <c r="I158" s="5" t="s">
         <v>16</v>
       </c>
@@ -9168,7 +9482,9 @@
       <c r="G159" s="3" t="s">
         <v>671</v>
       </c>
-      <c r="H159" s="3"/>
+      <c r="H159" s="3" t="s">
+        <v>945</v>
+      </c>
       <c r="I159" s="6" t="s">
         <v>398</v>
       </c>
@@ -9242,7 +9558,9 @@
       <c r="G161" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="H161" s="3"/>
+      <c r="H161" s="3" t="s">
+        <v>946</v>
+      </c>
       <c r="I161" s="6" t="s">
         <v>16</v>
       </c>
@@ -9278,7 +9596,9 @@
       <c r="G162" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="H162" s="4"/>
+      <c r="H162" s="4" t="s">
+        <v>946</v>
+      </c>
       <c r="I162" s="5" t="s">
         <v>16</v>
       </c>
@@ -9314,7 +9634,9 @@
       <c r="G163" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H163" s="3"/>
+      <c r="H163" s="3" t="s">
+        <v>947</v>
+      </c>
       <c r="I163" s="6" t="s">
         <v>16</v>
       </c>
@@ -9350,7 +9672,9 @@
       <c r="G164" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H164" s="4"/>
+      <c r="H164" s="4" t="s">
+        <v>947</v>
+      </c>
       <c r="I164" s="5" t="s">
         <v>398</v>
       </c>
@@ -9386,7 +9710,9 @@
       <c r="G165" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H165" s="3"/>
+      <c r="H165" s="3" t="s">
+        <v>947</v>
+      </c>
       <c r="I165" s="6" t="s">
         <v>16</v>
       </c>
@@ -9498,7 +9824,9 @@
       <c r="G168" s="4" t="s">
         <v>694</v>
       </c>
-      <c r="H168" s="4"/>
+      <c r="H168" s="4" t="s">
+        <v>948</v>
+      </c>
       <c r="I168" s="5" t="s">
         <v>16</v>
       </c>
@@ -9872,7 +10200,9 @@
       <c r="G178" s="4" t="s">
         <v>716</v>
       </c>
-      <c r="H178" s="4"/>
+      <c r="H178" s="4" t="s">
+        <v>949</v>
+      </c>
       <c r="I178" s="5" t="s">
         <v>16</v>
       </c>
@@ -9908,7 +10238,9 @@
       <c r="G179" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="H179" s="3"/>
+      <c r="H179" s="3" t="s">
+        <v>950</v>
+      </c>
       <c r="I179" s="6" t="s">
         <v>16</v>
       </c>
@@ -9944,7 +10276,9 @@
       <c r="G180" s="4" t="s">
         <v>722</v>
       </c>
-      <c r="H180" s="4"/>
+      <c r="H180" s="4" t="s">
+        <v>951</v>
+      </c>
       <c r="I180" s="5" t="s">
         <v>16</v>
       </c>
@@ -9980,7 +10314,9 @@
       <c r="G181" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="H181" s="3"/>
+      <c r="H181" s="3" t="s">
+        <v>952</v>
+      </c>
       <c r="I181" s="6" t="s">
         <v>16</v>
       </c>

</xml_diff>